<commit_message>
Update timesheet and delete useless React component
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Time Tracking/Timesheet.xlsx
+++ b/DOCUMENTATION/Time Tracking/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Desktop\CISC 4900 PROJECT\Documentation\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26897AFE-728F-4371-8BBC-E6DA2743A1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4270884-229A-40F8-81EE-55741C0EEA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Task Description</t>
   </si>
@@ -163,6 +163,27 @@
   </si>
   <si>
     <t>Technology Assessment: Assessing and selecting the most suitable technologies for app development.</t>
+  </si>
+  <si>
+    <t>09/18/2023 – 09/24/2023</t>
+  </si>
+  <si>
+    <t>Database Schema Expansion: Introduced two new schemas, 'photos' and 'languages,' to enhance database functionality.</t>
+  </si>
+  <si>
+    <t>Database Update: Integrated 'languages' into the database for expanded functionality.</t>
+  </si>
+  <si>
+    <t>Form Development Milestone: Successfully constructed login, registration, and profile creation forms.</t>
+  </si>
+  <si>
+    <t>Component Integration Research: Exploring npm documentation for seamless integration of desired components into my application.</t>
+  </si>
+  <si>
+    <t>Express App Route Documentation: Defining and documenting the application's routes for clarity and reference.</t>
+  </si>
+  <si>
+    <t>User Registration and Authentication Design Document: Crafting a comprehensive blueprint for routes and controllers.</t>
   </si>
 </sst>
 </file>
@@ -240,12 +261,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -539,18 +559,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="128.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" style="1" customWidth="1"/>
   </cols>
@@ -576,650 +596,738 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>45163</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0.11625000000000001</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>0.16553240740740741</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>45163</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2.7210648148148147E-2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>0.16553240740740741</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>45165</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>2.207175925925926E-2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>0.16553240740740741</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>45166</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.21519675925925927</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>45167</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>2.0752314814814814E-2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>45168</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>6.5509259259259262E-3</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>45168</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>5.5787037037037038E-3</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>45168</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>4.1273148148148149E-2</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>0.530787037037037</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>45170</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>2.8819444444444444E-3</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>45170</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>2.2569444444444447E-3</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>45170</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>6.5972222222222222E-3</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>45170</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>8.4155092592592587E-2</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>45171</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.34585648148148151</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>1.2618865740740741</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>45173</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0.16436342592592593</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>45174</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0.19474537037037035</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>45175</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>0.13197916666666668</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>45175</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>3.1377314814814809E-2</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>45175</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>6.0092592592592593E-2</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>45175</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>6.2199074074074073E-2</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>45176</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>6.5046296296296297E-2</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>45177</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>0.12812500000000002</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>45178</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>0.28138888888888891</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>45179</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>0.19888888888888889</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>45179</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>0.13437499999999999</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>1.4525810185185186</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>45180</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>0.39216435185185183</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>45181</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>0.2878472222222222</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F28" s="10"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>45182</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>0.14900462962962963</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F29" s="10"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>45182</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>2.0266203703703703E-2</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F30" s="10"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>45182</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>0.11255787037037036</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F31" s="10"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>45182</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>0.12630787037037036</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F32" s="10"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>45184</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>0.18487268518518518</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>45185</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>8.8668981481481488E-2</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>45186</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>3.0821759259259257E-2</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F35" s="10"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>45186</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>0.26060185185185186</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="10">
         <v>1.6531134259259259</v>
       </c>
-      <c r="F36" s="10"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="10"/>
+      <c r="A37" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="5">
+        <v>45187</v>
+      </c>
+      <c r="C37" s="6">
+        <v>7.9618055555555553E-2</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="10"/>
+      <c r="A38" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C38" s="6">
+        <v>3.0150462962962962E-2</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.13921296296296296</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C40" s="6">
+        <v>5.4780092592592589E-2</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C41" s="6">
+        <v>8.1597222222222227E-3</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="5">
+        <v>45189</v>
+      </c>
+      <c r="C42" s="6">
+        <v>9.8518518518518519E-2</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Introduce resetPassword and updatePassword controller functions; restrict updatePassword access to logged-in users.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Time Tracking/Timesheet.xlsx
+++ b/DOCUMENTATION/Time Tracking/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Desktop\CISC 4900 PROJECT\Documentation\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07299178-2DB0-46AE-B699-E6F3720C3B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E6906E-238F-4557-B4BE-884D0487E122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>